<commit_message>
Change from Enhanced REFramework to REFramework
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,31 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihai.dunareanu\Documents\UiPath\UiPath Enchanced REFramework\UiPath_REFramework\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA72E52-A4BE-4685-A33D-CE96D31DF1B7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11715" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Introduction" sheetId="7" r:id="rId1"/>
-    <sheet name="Settings" sheetId="1" r:id="rId2"/>
-    <sheet name="Credentials" sheetId="6" r:id="rId3"/>
-    <sheet name="Tasks" sheetId="5" r:id="rId4"/>
-    <sheet name="Constants" sheetId="2" r:id="rId5"/>
-    <sheet name="Assets" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Settings" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Constants" sheetId="2" r:id="rId4"/>
+    <sheet state="visible" name="Assets" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -33,12 +21,21 @@
     <t>Value</t>
   </si>
   <si>
+    <t>Asset</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
+    <t>Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
     <t>MaxRetryNumber</t>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with application exception. Must be integer</t>
+  </si>
+  <si>
     <t>TimeoutShort</t>
   </si>
   <si>
@@ -102,793 +99,139 @@
     <t>Image accuracy high value, for images that have low contrast. Must be double</t>
   </si>
   <si>
+    <t>LogMessage_GetTransactionData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionDataError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error getting transaction data for Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Error retrieving Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_Success</t>
+  </si>
+  <si>
+    <t>Transaction Successful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful</t>
+  </si>
+  <si>
+    <t>LogMessage_BusinessRuleException</t>
+  </si>
+  <si>
+    <t>Business rule exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception</t>
+  </si>
+  <si>
+    <t>LogMessage_ApplicationException</t>
+  </si>
+  <si>
+    <t>System exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
+    <t>KibanaDemoQueue</t>
+  </si>
+  <si>
     <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
   </si>
   <si>
-    <t>Asset</t>
-  </si>
-  <si>
-    <t>Description (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>ServicesLayer\FirstRun\</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The task that executes first time programs starts. Responsible for its own configuration, data, processing, and retires. The task name value is used by the program to obtian the path to the slave program's root folder, relative to the main program's.
-</t>
-  </si>
-  <si>
-    <t>Task path location</t>
-  </si>
-  <si>
-    <t>Key is the TaskName and value is the Task Environment (path)</t>
-  </si>
-  <si>
-    <t>SystemTask1_Env</t>
-  </si>
-  <si>
-    <t>SystemTask1_Enable</t>
-  </si>
-  <si>
-    <t>SystemTask2_Env</t>
-  </si>
-  <si>
-    <t>SystemTask2_Enable</t>
-  </si>
-  <si>
-    <t>ServicesLayer\GetData\</t>
-  </si>
-  <si>
-    <t>Enable Task setting. [0=Disable. 1=Enable during first run, 2=Always enable]</t>
-  </si>
-  <si>
-    <t>ServicesLayer\Task1</t>
-  </si>
-  <si>
-    <t>ServicesLayer\Task2</t>
-  </si>
-  <si>
-    <t>MaxInitRetryNumber</t>
-  </si>
-  <si>
-    <t>MaxContinuousRetryNumber</t>
-  </si>
-  <si>
-    <t>If &gt; 0 will retry the Initialisation state with a failed exception. Must be an integer.</t>
-  </si>
-  <si>
-    <t>If &gt; 0 will keep a record of consecutive failed exceptions of the Process state. When this number is reached, the application will fail. Must be an integer.</t>
-  </si>
-  <si>
-    <t>If &gt; 0, the robot will retry the same transaction which failed with application exception. This is a local data retry. Orchestrator Queue Item retry are managed at the queue level. Must be integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You may want to mark keys in this settings dictionary with certain colours. One use I've needed for colors was to define the keys needed in the operation of the framework. </t>
-  </si>
-  <si>
-    <t>This key belongs to user designated category 1</t>
-  </si>
-  <si>
-    <t>This key is used in the Framework layer. You can change the values, but do not delete the keys</t>
-  </si>
-  <si>
-    <t>This key is used in the Business Process Layer. The developer is responsible for the keys. The user is responsible for the values.</t>
-  </si>
-  <si>
-    <t>Help regarding this Configuration File</t>
-  </si>
-  <si>
-    <t>This is the configuration file used to describe various changeable parameters of the process. You should use this file to store settings that are environment related (like paths to programs or resources), user related (email account names, credential names), or plain data (URL of website or name of SAP report to execute). Below, the purpose of each sheet is explained in more detail.</t>
-  </si>
-  <si>
-    <t>Settings</t>
-  </si>
-  <si>
-    <t>Credentials</t>
-  </si>
-  <si>
-    <t>Tasks</t>
-  </si>
-  <si>
-    <t>Constants</t>
-  </si>
-  <si>
-    <t>Assets</t>
-  </si>
-  <si>
-    <t>The credentials sheet is the place to store your credential names.There is also one special credential, that needs to be defined only once, and which is comprised of the URL, TenancyName and CredentialName required to authenticate to the Orchestrator server using REST API. This is only used when working with QueueItems.</t>
-  </si>
-  <si>
-    <t>FirstRunTask: This task is invoked in the Framework Layer and executes only once(Even if Transaction number 1 were to fail and be retried, it would not be executed again), at program startup. It should not interact with data in memory, since it executes before we enter the main process data layer, but it can be used as a queue dispatcher.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task1: This task is not invoked anywhere, and should be used by the developer. </t>
-  </si>
-  <si>
-    <t>The sheet contains the list of tasks. Each task is another Business Process Layer context that is executed at some point during the main process execution. For system tasks, the execution is preselected and configurable from the settings. For user added tasks, it is chosen by the user.</t>
-  </si>
-  <si>
-    <t>GetDataTask: This task is invoked in the Data Layer of the main task. The reason is that we might desire it to deliver some TransactionData to us is a safe manner. Thus, it might navigate a website, download a file, process it, and deliver us an output datatable TransactionData. This would be made available in the Data Layer of the main task and would be ready for usage according to the business rules of the process.</t>
-  </si>
-  <si>
-    <t>This sheet is the place to store plain data, as well as most user data with the important exception of credential names.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typically there is not much for you to add here, although you want to check/change the settings of the Retry mechanism implemented in at the framework layer, during transaction processing, exception recovery, and continuous failiure. Also stores constants used throughout the program, like preconfiguered delays, timeouts. </t>
-  </si>
-  <si>
-    <t>This sheet is used to fetch assets from Orchestrator. The column name is the key, while the column asset hoolds the asset name in Orchestrator. If there is another local key with the same name, it will be overwritten by the value fetched from Orchestrator.</t>
-  </si>
-  <si>
-    <t>####  Legend of Key Value pair colours####</t>
-  </si>
-  <si>
-    <t>Enable the execution of the FirstRun Task. (0=disable, 1=enable)</t>
-  </si>
-  <si>
-    <t>This key belongs to user designated category 2</t>
-  </si>
-  <si>
-    <t>Task1_Env</t>
-  </si>
-  <si>
-    <t>Task2_Env</t>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="14.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
-  <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+  <cellXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Bad" xfId="4" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="2" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="3" builtinId="10"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4472C4"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358C8B53-A61E-4F05-B727-D34F2E27D989}">
-  <dimension ref="A1:A23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="118" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="68.0"/>
+    <col customWidth="1" min="2" max="2" width="70.14"/>
+    <col customWidth="1" min="3" max="3" width="68.57"/>
+    <col customWidth="1" min="4" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75">
-      <c r="A1" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="18.75">
-      <c r="A2" s="7"/>
-    </row>
-    <row r="3" spans="1:1" ht="60">
-      <c r="A3" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75">
-      <c r="A4" s="12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15.75">
-      <c r="A6" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="45">
-      <c r="A7" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15.75">
-      <c r="A8" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="45">
-      <c r="A9" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="45">
-      <c r="A10" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="60">
-      <c r="A11" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15.75">
-      <c r="A13" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="45">
-      <c r="A14" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="15.75">
-      <c r="A15" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="30">
-      <c r="A16" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="13"/>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="30">
-      <c r="A19" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z991"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,7 +239,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -922,17 +265,43 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1">
-      <c r="B3" s="3"/>
+    <row r="3" ht="14.25" customHeight="1"/>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
     </row>
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1"/>
@@ -1906,29 +1275,31 @@
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC672C-F735-4EF3-8287-9B35E6A7A36A}">
-  <dimension ref="A1:Z988"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="53.0"/>
+    <col customWidth="1" min="2" max="2" width="63.57"/>
+    <col customWidth="1" min="3" max="3" width="89.0"/>
+    <col customWidth="1" min="4" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1936,7 +1307,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1962,14 +1333,188 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="2" ht="14.25" customHeight="1"/>
+    <row r="3" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>5000.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>30000.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>120000.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1000.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>15000.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>60000.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>0.6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>0.8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>0.9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="24" ht="14.25" customHeight="1"/>
     <row r="25" ht="14.25" customHeight="1"/>
     <row r="26" ht="14.25" customHeight="1"/>
@@ -2935,133 +2480,42 @@
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E783D41C-6E2C-4977-A8D7-34F9BFEB9E5D}">
-  <dimension ref="A1:C8"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
+    <col customWidth="1" min="1" max="26" width="65.43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z998"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3087,1196 +2541,21 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>5000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>30000</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>120000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>1000</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>15000</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <v>60000</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <v>0.6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
-        <v>0.8</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17">
-        <v>0.9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="26" width="65.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" ht="14.25" customHeight="1"/>
+    <row r="3" ht="14.25" customHeight="1"/>
+    <row r="4" ht="14.25" customHeight="1"/>
+    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="6" ht="14.25" customHeight="1"/>
+    <row r="7" ht="14.25" customHeight="1"/>
+    <row r="8" ht="14.25" customHeight="1"/>
+    <row r="9" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1"/>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
+    <row r="15" ht="14.25" customHeight="1"/>
+    <row r="16" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -5262,6 +3541,6 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>